<commit_message>
Ajuste de la Queratina
% a Marinela
Menor % a los profesionales de Tocador
</commit_message>
<xml_diff>
--- a/0. Nomina/Info.xlsx
+++ b/0. Nomina/Info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\windows\Documents\GitHub\Problem_Set_1\ForeverChic\0. Nomina\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B37385-FD8C-42C9-9951-B4673437648C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B929BA4C-EE80-4E22-85FF-D2D2DF8900BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="1" xr2:uid="{E10BBF24-8B64-47E0-9392-E6A1EA239C1A}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="116">
   <si>
     <t>Blower  Cabello medio</t>
   </si>
@@ -1205,8 +1205,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{513E435A-5C6B-4ABF-A51B-E8068E26EF98}" name="Tabla4" displayName="Tabla4" ref="A1:A21" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="A1:A21" xr:uid="{513E435A-5C6B-4ABF-A51B-E8068E26EF98}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{513E435A-5C6B-4ABF-A51B-E8068E26EF98}" name="Tabla4" displayName="Tabla4" ref="A1:A19" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="A1:A19" xr:uid="{513E435A-5C6B-4ABF-A51B-E8068E26EF98}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{21692516-7C50-4234-9E59-8754AD7371D9}" name="Servicio" dataDxfId="22"/>
   </tableColumns>
@@ -1245,8 +1245,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{8F17279D-8BB3-4F47-BDA2-D4B0B503999D}" name="Tabla9" displayName="Tabla9" ref="A1:A8" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:A8" xr:uid="{8F17279D-8BB3-4F47-BDA2-D4B0B503999D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{8F17279D-8BB3-4F47-BDA2-D4B0B503999D}" name="Tabla9" displayName="Tabla9" ref="A1:A9" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:A9" xr:uid="{8F17279D-8BB3-4F47-BDA2-D4B0B503999D}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{98EAFF14-E836-4D53-B221-D8250D4DCB23}" name="Servicio" dataDxfId="10"/>
   </tableColumns>
@@ -1723,9 +1723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C0B312-857B-4CB8-9169-D3C16819EF41}">
   <dimension ref="B1:O123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7123,9 +7121,9 @@
       <c r="B121" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C121" s="13">
-        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla4[Servicio],0)&gt;=1,1,""),"")</f>
-        <v>1</v>
+      <c r="C121" s="13" t="str">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla4[Servicio],0)&gt;=1,1,""),"")</f>
+        <v/>
       </c>
       <c r="D121" s="13" t="str">
         <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla5[Servicio],0)&gt;=1,1,""),"")</f>
@@ -7139,9 +7137,9 @@
         <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla8[Servicio],0)&gt;=1,1,""),"")</f>
         <v/>
       </c>
-      <c r="G121" s="13" t="str">
-        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla9[Servicio],0)&gt;=1,1,""),"")</f>
-        <v/>
+      <c r="G121" s="13">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla9[Servicio],0)&gt;=1,1,""),"")</f>
+        <v>1</v>
       </c>
       <c r="H121" s="13" t="str">
         <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla10[Servicio],0)&gt;=1,1,""),"")</f>
@@ -7264,10 +7262,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCD82325-C883-442E-BAE1-2232B8CCAA6F}">
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A2:A21"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7358,27 +7356,17 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -7877,10 +7865,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4B6EF07-1B24-43F3-84D1-8FE766884035}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7927,6 +7915,11 @@
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajustes A la Nomina
* Pintar de Amarillo en los reportes
* Cambio en el Formato Fecha
* Entre Otros ....
</commit_message>
<xml_diff>
--- a/0. Nomina/Info.xlsx
+++ b/0. Nomina/Info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\windows\Documents\GitHub\Problem_Set_1\ForeverChic\0. Nomina\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B929BA4C-EE80-4E22-85FF-D2D2DF8900BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5539ACA3-D38A-4112-87AD-E13A13A61D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="1" xr2:uid="{E10BBF24-8B64-47E0-9392-E6A1EA239C1A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{E10BBF24-8B64-47E0-9392-E6A1EA239C1A}"/>
   </bookViews>
   <sheets>
     <sheet name="0. Profesionales" sheetId="10" r:id="rId1"/>
@@ -1573,7 +1573,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB14EE81-1336-48D1-AF56-B5F648183D15}">
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1723,7 +1725,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C0B312-857B-4CB8-9169-D3C16819EF41}">
   <dimension ref="B1:O123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Ajustes Nomina 15/30 NOV
Ajustes para la Nomina del 15/30 NOV
* Se cargo la base de datos completa
* Se modifico el codigo para que lea la base
* Se genero la base de descuentos para Color
* Se completo la Base de dotos INFO con los nuevos servicios y productos.
</commit_message>
<xml_diff>
--- a/0. Nomina/Info.xlsx
+++ b/0. Nomina/Info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\windows\Documents\GitHub\Problem_Set_1\ForeverChic\0. Nomina\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652C516F-76FD-448B-A139-4B32185149CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12096A3F-0883-414D-A1E7-B8C53B9DD5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="2" xr2:uid="{E10BBF24-8B64-47E0-9392-E6A1EA239C1A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="1" xr2:uid="{E10BBF24-8B64-47E0-9392-E6A1EA239C1A}"/>
   </bookViews>
   <sheets>
     <sheet name="0. Profesionales" sheetId="10" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="127">
   <si>
     <t>Blower  Cabello medio</t>
   </si>
@@ -416,6 +416,15 @@
   </si>
   <si>
     <t>Cuticle revitaizer oil</t>
+  </si>
+  <si>
+    <t>Balaca queratina desde</t>
+  </si>
+  <si>
+    <t>Essential Densifying lotion -  Caja de 12 unidades  por 7 Unidades</t>
+  </si>
+  <si>
+    <t>Scalego densifying Shampoo 300 ml</t>
   </si>
 </sst>
 </file>
@@ -1189,8 +1198,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{E5B4A5EC-23CC-4AAF-BBA4-AA33F630A4B6}" name="Tabla12" displayName="Tabla12" ref="B2:L131" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
-  <autoFilter ref="B2:L131" xr:uid="{E5B4A5EC-23CC-4AAF-BBA4-AA33F630A4B6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{E5B4A5EC-23CC-4AAF-BBA4-AA33F630A4B6}" name="Tabla12" displayName="Tabla12" ref="B2:L134" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+  <autoFilter ref="B2:L134" xr:uid="{E5B4A5EC-23CC-4AAF-BBA4-AA33F630A4B6}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{0AE342CE-E699-4674-A921-02F9F207D78B}" name="Servicio" dataDxfId="35"/>
     <tableColumn id="2" xr3:uid="{419527B9-DDA5-4A0B-905E-3A831C54499E}" name="1. Tocador" dataDxfId="34">
@@ -1269,8 +1278,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{8F17279D-8BB3-4F47-BDA2-D4B0B503999D}" name="Tabla9" displayName="Tabla9" ref="A1:A10" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:A10" xr:uid="{8F17279D-8BB3-4F47-BDA2-D4B0B503999D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{8F17279D-8BB3-4F47-BDA2-D4B0B503999D}" name="Tabla9" displayName="Tabla9" ref="A1:A11" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:A11" xr:uid="{8F17279D-8BB3-4F47-BDA2-D4B0B503999D}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{98EAFF14-E836-4D53-B221-D8250D4DCB23}" name="Servicio" dataDxfId="10"/>
   </tableColumns>
@@ -1279,8 +1288,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4BF8DC9D-BBFD-4565-9457-5C2CBB709635}" name="Tabla10" displayName="Tabla10" ref="A1:A12" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:A12" xr:uid="{4BF8DC9D-BBFD-4565-9457-5C2CBB709635}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4BF8DC9D-BBFD-4565-9457-5C2CBB709635}" name="Tabla10" displayName="Tabla10" ref="A1:A14" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:A14" xr:uid="{4BF8DC9D-BBFD-4565-9457-5C2CBB709635}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{DB57ABA3-E3AD-4F77-B798-6C0D142D72DC}" name="Servicio" dataDxfId="7"/>
   </tableColumns>
@@ -1747,11 +1756,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C0B312-857B-4CB8-9169-D3C16819EF41}">
-  <dimension ref="B1:O131"/>
+  <dimension ref="B1:O134"/>
   <sheetViews>
-    <sheetView topLeftCell="A114" workbookViewId="0">
-      <selection activeCell="B129" sqref="B129"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7640,6 +7647,141 @@
         <v/>
       </c>
     </row>
+    <row r="132" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B132" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C132" s="13" t="str">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla4[Servicio],0)&gt;=1,1,""),"")</f>
+        <v/>
+      </c>
+      <c r="D132" s="13" t="str">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla5[Servicio],0)&gt;=1,1,""),"")</f>
+        <v/>
+      </c>
+      <c r="E132" s="13" t="str">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla6[Servicio],0)&gt;=1,1,""),"")</f>
+        <v/>
+      </c>
+      <c r="F132" s="13" t="str">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla8[Servicio],0)&gt;=1,1,""),"")</f>
+        <v/>
+      </c>
+      <c r="G132" s="13">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla9[Servicio],0)&gt;=1,1,""),"")</f>
+        <v>1</v>
+      </c>
+      <c r="H132" s="13" t="str">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla10[Servicio],0)&gt;=1,1,""),"")</f>
+        <v/>
+      </c>
+      <c r="I132" s="13" t="str">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla11[Servicio],0)&gt;=1,1,""),"")</f>
+        <v/>
+      </c>
+      <c r="J132" s="13" t="str">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla2[Servicio],0)&gt;=1,1,""),"")</f>
+        <v/>
+      </c>
+      <c r="K132" s="13" t="str">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla7[Servicio],0)&gt;=1,1,""),"")</f>
+        <v/>
+      </c>
+      <c r="L132" s="17" t="str">
+        <f>IF(SUM(Tabla12[[#This Row],[1. Tocador]:[9. Accesorios]])=1,"","❎")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="133" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B133" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C133" s="13" t="str">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla4[Servicio],0)&gt;=1,1,""),"")</f>
+        <v/>
+      </c>
+      <c r="D133" s="13" t="str">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla5[Servicio],0)&gt;=1,1,""),"")</f>
+        <v/>
+      </c>
+      <c r="E133" s="13" t="str">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla6[Servicio],0)&gt;=1,1,""),"")</f>
+        <v/>
+      </c>
+      <c r="F133" s="13" t="str">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla8[Servicio],0)&gt;=1,1,""),"")</f>
+        <v/>
+      </c>
+      <c r="G133" s="13" t="str">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla9[Servicio],0)&gt;=1,1,""),"")</f>
+        <v/>
+      </c>
+      <c r="H133" s="13">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla10[Servicio],0)&gt;=1,1,""),"")</f>
+        <v>1</v>
+      </c>
+      <c r="I133" s="13" t="str">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla11[Servicio],0)&gt;=1,1,""),"")</f>
+        <v/>
+      </c>
+      <c r="J133" s="13" t="str">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla2[Servicio],0)&gt;=1,1,""),"")</f>
+        <v/>
+      </c>
+      <c r="K133" s="13" t="str">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla7[Servicio],0)&gt;=1,1,""),"")</f>
+        <v/>
+      </c>
+      <c r="L133" s="17" t="str">
+        <f>IF(SUM(Tabla12[[#This Row],[1. Tocador]:[9. Accesorios]])=1,"","❎")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="134" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B134" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="C134" s="13" t="str">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla4[Servicio],0)&gt;=1,1,""),"")</f>
+        <v/>
+      </c>
+      <c r="D134" s="13" t="str">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla5[Servicio],0)&gt;=1,1,""),"")</f>
+        <v/>
+      </c>
+      <c r="E134" s="13" t="str">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla6[Servicio],0)&gt;=1,1,""),"")</f>
+        <v/>
+      </c>
+      <c r="F134" s="13" t="str">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla8[Servicio],0)&gt;=1,1,""),"")</f>
+        <v/>
+      </c>
+      <c r="G134" s="13" t="str">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla9[Servicio],0)&gt;=1,1,""),"")</f>
+        <v/>
+      </c>
+      <c r="H134" s="13">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla10[Servicio],0)&gt;=1,1,""),"")</f>
+        <v>1</v>
+      </c>
+      <c r="I134" s="13" t="str">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla11[Servicio],0)&gt;=1,1,""),"")</f>
+        <v/>
+      </c>
+      <c r="J134" s="13" t="str">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla2[Servicio],0)&gt;=1,1,""),"")</f>
+        <v/>
+      </c>
+      <c r="K134" s="13" t="str">
+        <f>IFERROR(IF(MATCH(Tabla12[[#This Row],[Servicio]],Tabla7[Servicio],0)&gt;=1,1,""),"")</f>
+        <v/>
+      </c>
+      <c r="L134" s="17" t="str">
+        <f>IF(SUM(Tabla12[[#This Row],[1. Tocador]:[9. Accesorios]])=1,"","❎")</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -7652,7 +7794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCD82325-C883-442E-BAE1-2232B8CCAA6F}">
   <dimension ref="A1:A20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8281,10 +8423,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4B6EF07-1B24-43F3-84D1-8FE766884035}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8343,6 +8485,11 @@
         <v>119</v>
       </c>
     </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -8353,10 +8500,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50A6DBDC-6E11-4A4A-8118-90EDBF21AE1E}">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8423,6 +8570,16 @@
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>